<commit_message>
updated examples in D3_all_vaccines_curated and  D3_study_population_target_cohorts
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_all_vaccines_curated.xlsx
+++ b/i_codebooks/D3_all_vaccines_curated.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>medatata_name</t>
   </si>
@@ -151,9 +151,6 @@
     <t>P003</t>
   </si>
   <si>
-    <t>P004</t>
-  </si>
-  <si>
     <t>persons in the instance</t>
   </si>
   <si>
@@ -184,22 +181,19 @@
     <t>COV</t>
   </si>
   <si>
-    <t>TET</t>
-  </si>
-  <si>
-    <t>DIP</t>
-  </si>
-  <si>
-    <t>PER</t>
-  </si>
-  <si>
-    <t>same</t>
-  </si>
-  <si>
     <t>D3_all_vaccines_curated</t>
   </si>
   <si>
-    <t>these 3 records are originated from the same original record of a trivalent vaccination</t>
+    <t>DIP-PER-TET</t>
+  </si>
+  <si>
+    <t>HPV</t>
+  </si>
+  <si>
+    <t>astrazeneca</t>
+  </si>
+  <si>
+    <t>moderna</t>
   </si>
 </sst>
 </file>
@@ -291,7 +285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -434,73 +428,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -556,42 +488,9 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -931,7 +830,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -939,7 +838,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -947,7 +846,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
@@ -955,7 +854,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -963,7 +862,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -971,7 +870,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -979,7 +878,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1084,7 +983,7 @@
         <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s">
         <v>24</v>
@@ -1103,16 +1002,16 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
         <v>24</v>
@@ -1217,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1229,10 +1128,10 @@
     <col min="2" max="2" width="12.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>20</v>
       </c>
@@ -1246,236 +1145,157 @@
         <v>30</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="21">
-        <v>44197</v>
-      </c>
-      <c r="C2" s="20">
+      <c r="B2" s="24">
+        <v>44318</v>
+      </c>
+      <c r="C2" s="23">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="24">
+        <v>44404</v>
+      </c>
+      <c r="C3" s="23">
+        <v>2</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="28">
+        <v>44428</v>
+      </c>
+      <c r="C4" s="27">
+        <v>1</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="21">
-        <v>44221</v>
-      </c>
-      <c r="C3" s="20">
+      <c r="E4" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="21">
+        <v>44407</v>
+      </c>
+      <c r="C5" s="20">
         <v>2</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="21">
-        <v>44287</v>
-      </c>
-      <c r="C4" s="20">
-        <v>3</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="21">
-        <v>44359</v>
-      </c>
-      <c r="C5" s="20">
-        <v>4</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="24">
-        <v>44428</v>
-      </c>
-      <c r="C6" s="23">
+      <c r="B6" s="21">
+        <v>44772</v>
+      </c>
+      <c r="C6" s="20">
         <v>1</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="20"/>
+      <c r="E6" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="24">
+        <v>44197</v>
+      </c>
+      <c r="C7" s="23">
+        <v>1</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="24">
+        <v>44221</v>
+      </c>
+      <c r="C8" s="23">
+        <v>2</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="24">
+        <v>44287</v>
+      </c>
+      <c r="C9" s="23">
+        <v>3</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="E9" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="21">
-        <v>44407</v>
-      </c>
-      <c r="C7" s="20">
-        <v>1</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="24">
-        <v>44318</v>
-      </c>
-      <c r="C8" s="23">
-        <v>1</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="34"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="24">
-        <v>44318</v>
-      </c>
-      <c r="C9" s="23">
-        <v>1</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="36"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
-        <v>38</v>
-      </c>
       <c r="B10" s="24">
-        <v>44318</v>
+        <v>44481</v>
       </c>
       <c r="C10" s="23">
-        <v>1</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="24">
-        <v>44404</v>
-      </c>
-      <c r="C11" s="23">
-        <v>2</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="28"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="24">
-        <v>44404</v>
-      </c>
-      <c r="C12" s="23">
-        <v>2</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="24">
-        <v>44404</v>
-      </c>
-      <c r="C13" s="23">
-        <v>2</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="32"/>
+      <c r="E10" s="25" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F8:G10"/>
-    <mergeCell ref="F11:G13"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1732,6 +1552,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
@@ -1741,15 +1570,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1772,6 +1592,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8A1FD8-B49B-4DD5-B035-18D91695717A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -1786,12 +1614,4 @@
     <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed type in D3_curated_all_vaccines
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_all_vaccines_curated.xlsx
+++ b/i_codebooks/D3_all_vaccines_curated.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -348,9 +348,6 @@
     <t>root indicators for all persons in the instance</t>
   </si>
   <si>
-    <t>as many as thedoses for that root_indicator, including duplicates</t>
-  </si>
-  <si>
     <t>NxUoO</t>
   </si>
   <si>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>This dataset contains the records of all the curated doses of all roots of indicators in the instance listed in Table 7 of the SAP. Doses of covid vaccines are included. It is obtained by D3_clean_all_vaccines by excluding records that are duplicates or of bad quality, and after appending the curated covid vaccines</t>
+  </si>
+  <si>
+    <t>as many as thedoses for that root_indicator</t>
   </si>
 </sst>
 </file>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1037,12 +1037,12 @@
         <v>6</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
@@ -1053,7 +1053,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
@@ -1076,10 +1076,10 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1511,7 +1511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1725,6 +1725,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -1975,15 +1984,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1997,6 +1997,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93CB37C0-20D2-41C5-B1FB-AE3E189FB0ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2011,14 +2019,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E3594D7-89C9-4FB7-87F1-388B97141296}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>